<commit_message>
added part visual feature
</commit_message>
<xml_diff>
--- a/GYM.xlsx
+++ b/GYM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Han Sun\Google Drive\Misc_Fun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Han Sun\Google Drive\Misc_Fun\workout_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682ADF8F-2EC9-4C66-9FC2-A53BB678BAEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE099AD0-C630-451A-935B-B63E7FDCB43F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week#1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="54">
   <si>
     <t>部位</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>Arm</t>
+  </si>
+  <si>
+    <t>SUM</t>
   </si>
 </sst>
 </file>
@@ -597,8 +600,8 @@
   </sheetPr>
   <dimension ref="A1:G240"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -764,6 +767,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G8">
         <f>SUM(G2:G7)</f>
         <v>10900</v>
@@ -906,6 +912,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G17">
         <f>SUM(G10:G16)</f>
         <v>15600</v>
@@ -1099,6 +1108,9 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G28">
         <f>SUM(G19:G27)</f>
         <v>15000</v>
@@ -1331,7 +1343,9 @@
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
+      <c r="B40" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
@@ -1554,8 +1568,8 @@
   </sheetPr>
   <dimension ref="A1:G240"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1721,6 +1735,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G8">
         <f>SUM(G2:G7)</f>
         <v>9788</v>
@@ -1863,6 +1880,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G17">
         <f>SUM(G10:G16)</f>
         <v>10600</v>
@@ -2055,6 +2075,9 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G28">
         <f>SUM(G19:G27)</f>
         <v>18544</v>
@@ -2278,6 +2301,9 @@
       </c>
     </row>
     <row r="40" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G40">
         <f>SUM(G30:G39)</f>
         <v>8250</v>
@@ -2495,8 +2521,8 @@
   </sheetPr>
   <dimension ref="A1:G240"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2662,6 +2688,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G8">
         <f>SUM(G2:G7)</f>
         <v>8456</v>
@@ -2702,6 +2731,15 @@
       <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
       <c r="G11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2813,6 +2851,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G17">
         <f>SUM(G10:G16)</f>
         <v>15400</v>
@@ -3005,6 +3046,9 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G28">
         <f>SUM(G19:G27)</f>
         <v>12400</v>
@@ -3228,6 +3272,9 @@
       </c>
     </row>
     <row r="40" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G40">
         <f>SUM(G30:G39)</f>
         <v>7860</v>
@@ -3445,8 +3492,8 @@
   </sheetPr>
   <dimension ref="A1:G240"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3612,6 +3659,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G8">
         <f>SUM(G2:G7)</f>
         <v>10820</v>
@@ -3652,6 +3702,15 @@
       <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
       <c r="G11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3763,6 +3822,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G17">
         <f>SUM(G10:G16)</f>
         <v>16800</v>
@@ -3911,6 +3973,12 @@
       <c r="D25" s="2">
         <v>0</v>
       </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
       <c r="G25" s="2">
         <v>0</v>
       </c>
@@ -3958,6 +4026,9 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G28">
         <f>SUM(G19:G27)</f>
         <v>16688</v>
@@ -4181,6 +4252,9 @@
       </c>
     </row>
     <row r="40" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G40">
         <f>SUM(G30:G39)</f>
         <v>8150</v>
@@ -4398,8 +4472,8 @@
   </sheetPr>
   <dimension ref="A1:G240"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4487,7 +4561,9 @@
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
       <c r="E4" s="2">
         <v>95</v>
       </c>
@@ -4563,6 +4639,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G8">
         <f>SUM(G2:G7)</f>
         <v>8858</v>
@@ -4603,6 +4682,15 @@
       <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
       <c r="G11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4657,7 +4745,9 @@
       <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
       <c r="E14" s="2">
         <v>45</v>
       </c>
@@ -4697,7 +4787,9 @@
       <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
       <c r="E16" s="2">
         <v>40</v>
       </c>
@@ -4710,6 +4802,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G17">
         <f>SUM(G10:G16)</f>
         <v>15000</v>
@@ -4750,7 +4845,9 @@
       <c r="C20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
       <c r="E20" s="2">
         <v>134</v>
       </c>
@@ -4790,7 +4887,9 @@
       <c r="C22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
       <c r="E22" s="2">
         <v>140</v>
       </c>
@@ -4901,6 +5000,9 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G28">
         <f>SUM(G19:G27)</f>
         <v>16500</v>
@@ -4941,7 +5043,9 @@
       <c r="C31" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
       <c r="E31" s="2">
         <v>50</v>
       </c>
@@ -4960,7 +5064,9 @@
       <c r="C32" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="2"/>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
       <c r="E32" s="2">
         <v>40</v>
       </c>
@@ -5120,6 +5226,9 @@
       </c>
     </row>
     <row r="40" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G40">
         <f>SUM(G30:G39)</f>
         <v>5400</v>
@@ -5337,8 +5446,8 @@
   </sheetPr>
   <dimension ref="A1:G240"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5426,7 +5535,9 @@
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
       <c r="E4" s="2">
         <v>95</v>
       </c>
@@ -5502,6 +5613,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G8">
         <f>SUM(G2:G7)</f>
         <v>9480</v>
@@ -5542,6 +5656,15 @@
       <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
       <c r="G11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5617,7 +5740,9 @@
       <c r="C15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
       <c r="E15" s="2">
         <v>140</v>
       </c>
@@ -5636,7 +5761,9 @@
       <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
       <c r="E16" s="2">
         <v>40</v>
       </c>
@@ -5649,6 +5776,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G17">
         <f>SUM(G10:G16)</f>
         <v>12800</v>
@@ -5689,7 +5819,9 @@
       <c r="C20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
       <c r="E20" s="2">
         <v>134</v>
       </c>
@@ -5771,7 +5903,9 @@
       <c r="C24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
       <c r="E24" s="2">
         <v>80</v>
       </c>
@@ -5793,6 +5927,12 @@
       <c r="D25" s="2">
         <v>0</v>
       </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
       <c r="G25" s="2">
         <v>0</v>
       </c>
@@ -5840,6 +5980,9 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G28">
         <f>SUM(G19:G27)</f>
         <v>22380</v>
@@ -5880,7 +6023,9 @@
       <c r="C31" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
       <c r="E31" s="2">
         <v>50</v>
       </c>
@@ -5899,7 +6044,9 @@
       <c r="C32" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="2"/>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
       <c r="E32" s="2">
         <v>40</v>
       </c>
@@ -6059,6 +6206,9 @@
       </c>
     </row>
     <row r="40" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G40">
         <f>SUM(G30:G39)</f>
         <v>5400</v>
@@ -6276,8 +6426,8 @@
   </sheetPr>
   <dimension ref="A1:G240"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6365,7 +6515,9 @@
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
       <c r="E4" s="2">
         <v>95</v>
       </c>
@@ -6441,6 +6593,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G8">
         <f>SUM(G2:G7)</f>
         <v>9760</v>
@@ -6481,6 +6636,9 @@
       <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
       <c r="G11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -6535,7 +6693,9 @@
       <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
       <c r="E14" s="2">
         <v>45</v>
       </c>
@@ -6588,6 +6748,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G17">
         <f>SUM(G10:G16)</f>
         <v>14580</v>
@@ -6628,7 +6791,9 @@
       <c r="C20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
       <c r="E20" s="2">
         <v>134</v>
       </c>
@@ -6647,7 +6812,9 @@
       <c r="C21" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
       <c r="E21" s="2">
         <v>90</v>
       </c>
@@ -6708,7 +6875,9 @@
       <c r="C24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
       <c r="E24" s="2">
         <v>80</v>
       </c>
@@ -6777,6 +6946,9 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G28">
         <f>SUM(G19:G27)</f>
         <v>16360</v>
@@ -6817,7 +6989,9 @@
       <c r="C31" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
       <c r="E31" s="2">
         <v>50</v>
       </c>
@@ -6983,7 +7157,9 @@
       <c r="C39" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D39" s="2"/>
+      <c r="D39" s="2">
+        <v>0</v>
+      </c>
       <c r="E39" s="2">
         <v>35</v>
       </c>
@@ -6996,6 +7172,9 @@
       </c>
     </row>
     <row r="40" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G40">
         <f>SUM(G30:G39)</f>
         <v>7200</v>
@@ -7213,8 +7392,8 @@
   </sheetPr>
   <dimension ref="A1:G240"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7281,7 +7460,9 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
       <c r="E3" s="2">
         <v>75</v>
       </c>
@@ -7300,7 +7481,9 @@
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
       <c r="E4" s="2">
         <v>95</v>
       </c>
@@ -7376,6 +7559,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G8">
         <f>SUM(G2:G7)</f>
         <v>6893</v>
@@ -7416,6 +7602,9 @@
       <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
       <c r="G11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7470,7 +7659,9 @@
       <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
       <c r="E14" s="2">
         <v>45</v>
       </c>
@@ -7510,7 +7701,9 @@
       <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
       <c r="E16" s="2">
         <v>40</v>
       </c>
@@ -7523,6 +7716,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G17">
         <f>SUM(G10:G16)</f>
         <v>15000</v>
@@ -7563,7 +7759,9 @@
       <c r="C20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
       <c r="E20" s="2">
         <v>134</v>
       </c>
@@ -7603,7 +7801,9 @@
       <c r="C22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
       <c r="E22" s="2">
         <v>145</v>
       </c>
@@ -7714,6 +7914,9 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G28">
         <f>SUM(G19:G27)</f>
         <v>18630</v>
@@ -7817,7 +8020,9 @@
       <c r="C34" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="2"/>
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
       <c r="E34" s="2">
         <v>40</v>
       </c>
@@ -7899,7 +8104,9 @@
       <c r="C38" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D38" s="2"/>
+      <c r="D38" s="2">
+        <v>0</v>
+      </c>
       <c r="E38" s="2">
         <v>30</v>
       </c>
@@ -7918,7 +8125,9 @@
       <c r="C39" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D39" s="2"/>
+      <c r="D39" s="2">
+        <v>0</v>
+      </c>
       <c r="E39" s="2">
         <v>35</v>
       </c>
@@ -7931,6 +8140,9 @@
       </c>
     </row>
     <row r="40" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G40">
         <f>SUM(G30:G39)</f>
         <v>7400</v>
@@ -8148,8 +8360,8 @@
   </sheetPr>
   <dimension ref="A1:G240"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8192,7 +8404,9 @@
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
       <c r="E2" s="2">
         <v>25</v>
       </c>
@@ -8214,7 +8428,9 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
       <c r="E3" s="2">
         <v>75</v>
       </c>
@@ -8233,7 +8449,9 @@
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
       <c r="E4" s="2">
         <v>95</v>
       </c>
@@ -8252,7 +8470,9 @@
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
       <c r="E5" s="2">
         <v>94</v>
       </c>
@@ -8271,7 +8491,9 @@
       <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
       <c r="E6" s="2">
         <v>65</v>
       </c>
@@ -8290,7 +8512,9 @@
       <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
       <c r="E7" s="2">
         <v>60</v>
       </c>
@@ -8303,6 +8527,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G8">
         <f>SUM(G2:G7)</f>
         <v>0</v>
@@ -8319,7 +8546,9 @@
       <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
       <c r="E10" s="2">
         <v>105</v>
       </c>
@@ -8341,6 +8570,15 @@
       <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
       <c r="G11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8353,7 +8591,9 @@
       <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
       <c r="E12" s="2">
         <v>80</v>
       </c>
@@ -8372,7 +8612,9 @@
       <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
       <c r="E13" s="2">
         <v>85</v>
       </c>
@@ -8391,7 +8633,9 @@
       <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
       <c r="E14" s="2">
         <v>45</v>
       </c>
@@ -8410,7 +8654,9 @@
       <c r="C15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
       <c r="E15" s="2">
         <v>140</v>
       </c>
@@ -8429,7 +8675,9 @@
       <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
       <c r="E16" s="2">
         <v>40</v>
       </c>
@@ -8442,6 +8690,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G17">
         <f>SUM(G10:G16)</f>
         <v>0</v>
@@ -8458,7 +8709,9 @@
       <c r="C19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
       <c r="E19" s="2">
         <v>174</v>
       </c>
@@ -8480,7 +8733,9 @@
       <c r="C20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
       <c r="E20" s="2">
         <v>134</v>
       </c>
@@ -8499,7 +8754,9 @@
       <c r="C21" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
       <c r="E21" s="2">
         <v>90</v>
       </c>
@@ -8518,7 +8775,9 @@
       <c r="C22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
       <c r="E22" s="2">
         <v>145</v>
       </c>
@@ -8537,7 +8796,9 @@
       <c r="C23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
       <c r="E23" s="2">
         <v>140</v>
       </c>
@@ -8556,7 +8817,9 @@
       <c r="C24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
       <c r="E24" s="2">
         <v>80</v>
       </c>
@@ -8575,7 +8838,9 @@
       <c r="C25" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
       <c r="G25" s="2">
         <v>0</v>
       </c>
@@ -8587,7 +8852,9 @@
       <c r="C26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="2"/>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
       <c r="E26" s="2">
         <v>90</v>
       </c>
@@ -8606,7 +8873,9 @@
       <c r="C27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
       <c r="E27" s="2">
         <v>40</v>
       </c>
@@ -8619,6 +8888,9 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G28">
         <f>SUM(G19:G27)</f>
         <v>0</v>
@@ -8635,7 +8907,9 @@
       <c r="C30" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="2"/>
+      <c r="D30" s="2">
+        <v>0</v>
+      </c>
       <c r="E30" s="2">
         <v>60</v>
       </c>
@@ -8657,7 +8931,9 @@
       <c r="C31" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
       <c r="E31" s="2">
         <v>50</v>
       </c>
@@ -8676,7 +8952,9 @@
       <c r="C32" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="2"/>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
       <c r="E32" s="2">
         <v>40</v>
       </c>
@@ -8695,7 +8973,9 @@
       <c r="C33" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D33" s="2"/>
+      <c r="D33" s="2">
+        <v>0</v>
+      </c>
       <c r="E33" s="2">
         <v>37.5</v>
       </c>
@@ -8714,7 +8994,9 @@
       <c r="C34" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="2"/>
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
       <c r="E34" s="2">
         <v>40</v>
       </c>
@@ -8733,7 +9015,9 @@
       <c r="C35" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="2"/>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
       <c r="E35" s="2">
         <v>0</v>
       </c>
@@ -8752,7 +9036,9 @@
       <c r="C36" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D36" s="2"/>
+      <c r="D36" s="2">
+        <v>0</v>
+      </c>
       <c r="E36" s="2">
         <v>35</v>
       </c>
@@ -8771,7 +9057,9 @@
       <c r="C37" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="2"/>
+      <c r="D37" s="2">
+        <v>0</v>
+      </c>
       <c r="E37" s="2">
         <v>35</v>
       </c>
@@ -8790,7 +9078,9 @@
       <c r="C38" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D38" s="2"/>
+      <c r="D38" s="2">
+        <v>0</v>
+      </c>
       <c r="E38" s="2">
         <v>30</v>
       </c>
@@ -8809,7 +9099,9 @@
       <c r="C39" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D39" s="2"/>
+      <c r="D39" s="2">
+        <v>0</v>
+      </c>
       <c r="E39" s="2">
         <v>35</v>
       </c>
@@ -8822,6 +9114,9 @@
       </c>
     </row>
     <row r="40" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G40">
         <f>SUM(G30:G39)</f>
         <v>0</v>

</xml_diff>